<commit_message>
add one more treemap level (region)
</commit_message>
<xml_diff>
--- a/data/GB_Einzel_Template_B2020.xlsx
+++ b/data/GB_Einzel_Template_B2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/sm16a062_campus_unibe_ch/Documents/FS22_OpenData_Übung/Projekt_Agro_Income/agro_income/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaeg\OneDrive - Universitaet Bern\FS22_OpenData_Übung\Projekt_Agro_Income\agro_income\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_0A1FD63016B7822A5AD1E4668DA695E592E362EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7216E56-5524-492A-91FD-C84DBF276614}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87061E32-77A7-462A-8EEF-C940B39E5221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1695" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZA-Data" sheetId="2" r:id="rId1"/>
@@ -9342,7 +9342,7 @@
   </sheetPr>
   <dimension ref="A1:BG682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AP419" workbookViewId="0">
       <selection activeCell="AX59" sqref="AX59"/>
     </sheetView>
   </sheetViews>
@@ -9350,8 +9350,9 @@
   <cols>
     <col min="1" max="53" width="10" style="1"/>
     <col min="54" max="54" width="2.375" style="1" customWidth="1"/>
-    <col min="55" max="56" width="10" style="1"/>
-    <col min="57" max="57" width="1.375" style="1" customWidth="1"/>
+    <col min="55" max="55" width="10" style="1"/>
+    <col min="56" max="56" width="26.5" style="1" customWidth="1"/>
+    <col min="57" max="57" width="45" style="1" customWidth="1"/>
     <col min="58" max="58" width="18.125" style="1" customWidth="1"/>
     <col min="59" max="16384" width="10" style="1"/>
   </cols>

</xml_diff>